<commit_message>
Spring boot guildelines V1.0
</commit_message>
<xml_diff>
--- a/doc/guideline/Spring Boot Guildeline.xlsx
+++ b/doc/guideline/Spring Boot Guildeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Github\word-of-the-day\doc\guideline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2219C6B0-953A-4FA9-A6BA-EEF8FACC66F8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06BDA3B-95F0-4825-84C7-D277611DBEC8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{05170AB7-19F1-440A-A5B4-C320B7BBF36E}"/>
   </bookViews>
@@ -516,9 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF32CE6-9F29-4850-8E42-E7F0EFE24732}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="AN133" sqref="AN133"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>